<commit_message>
added precision and acuracy values
</commit_message>
<xml_diff>
--- a/Micropipette Presentation.xlsx
+++ b/Micropipette Presentation.xlsx
@@ -5,15 +5,17 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fahad\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fahad\Documents\Git Bash\micropipette\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9885"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9885" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Drift Test" sheetId="1" r:id="rId1"/>
+    <sheet name="200uL" sheetId="2" r:id="rId2"/>
+    <sheet name="20uL" sheetId="3" r:id="rId3"/>
+    <sheet name="50uL" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="8">
   <si>
     <t>Amount Dispensed Experimental (1mL)Pipette (g)</t>
   </si>
@@ -34,6 +36,21 @@
   </si>
   <si>
     <t>Standard Deviation</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Percent Error</t>
+  </si>
+  <si>
+    <t>Percent Standard Deviation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Commercial </t>
   </si>
 </sst>
 </file>
@@ -267,7 +284,7 @@
           </c:trendline>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$51</c:f>
+              <c:f>'Drift Test'!$A$2:$A$51</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="50"/>
@@ -434,11 +451,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1910816032"/>
-        <c:axId val="1910812768"/>
+        <c:axId val="-433017392"/>
+        <c:axId val="-433023920"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1910816032"/>
+        <c:axId val="-433017392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -555,12 +572,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1910812768"/>
+        <c:crossAx val="-433023920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1910812768"/>
+        <c:axId val="-433023920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.19000000000000003"/>
@@ -679,7 +696,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1910816032"/>
+        <c:crossAx val="-433017392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -813,7 +830,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$51</c:f>
+              <c:f>'Drift Test'!$A$2:$A$51</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="50"/>
@@ -972,7 +989,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$51</c:f>
+              <c:f>'Drift Test'!$B$2:$B$51</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="50"/>
@@ -1139,11 +1156,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1740735088"/>
-        <c:axId val="1740726384"/>
+        <c:axId val="-433016848"/>
+        <c:axId val="-433023376"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1740735088"/>
+        <c:axId val="-433016848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1200,12 +1217,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1740726384"/>
+        <c:crossAx val="-433023376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1740726384"/>
+        <c:axId val="-433023376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1262,7 +1279,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1740735088"/>
+        <c:crossAx val="-433016848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2753,8 +2770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A69" sqref="A69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3243,12 +3260,483 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="13.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1">
+        <f>0.2*0.99997</f>
+        <v>0.19999400000000001</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0.20280000000000001</v>
+      </c>
+      <c r="B2">
+        <v>0.19289999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0.2044</v>
+      </c>
+      <c r="B3">
+        <v>0.1928</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0.2014</v>
+      </c>
+      <c r="B4">
+        <v>0.19220000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0.20039999999999999</v>
+      </c>
+      <c r="B5">
+        <v>0.2072</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>0.20100000000000001</v>
+      </c>
+      <c r="B6">
+        <v>0.19939999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>0.20519999999999999</v>
+      </c>
+      <c r="B7">
+        <v>0.19239999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>0.2082</v>
+      </c>
+      <c r="B8">
+        <v>0.2001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>0.20649999999999999</v>
+      </c>
+      <c r="B9">
+        <v>0.19969999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>0.20749999999999999</v>
+      </c>
+      <c r="B10">
+        <v>0.19950000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>0.2072</v>
+      </c>
+      <c r="B11">
+        <v>0.19620000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f>AVERAGE(A2:A11)</f>
+        <v>0.20446</v>
+      </c>
+      <c r="B12">
+        <f>AVERAGE(B2:B11)</f>
+        <v>0.19723999999999997</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f>STDEV(A2:A11)</f>
+        <v>2.9063914242770344E-3</v>
+      </c>
+      <c r="B13">
+        <f>STDEV(B2:B11)</f>
+        <v>4.849558971929532E-3</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f>((A12-(C1))/(C1))*100</f>
+        <v>2.2330669920097592</v>
+      </c>
+      <c r="B14">
+        <f>(B12-C1)/(C1)*100</f>
+        <v>-1.3770413112393542</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f>A13*100/A12</f>
+        <v>1.4214963436745742</v>
+      </c>
+      <c r="B15">
+        <f>B13*100/B12</f>
+        <v>2.4587096795424519</v>
+      </c>
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1">
+        <f>0.02*0.99997</f>
+        <v>1.9999400000000001E-2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1.9800000000000002E-2</v>
+      </c>
+      <c r="B2">
+        <v>1.9199999999999998E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1.9599999999999999E-2</v>
+      </c>
+      <c r="B3">
+        <v>1.9E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0.02</v>
+      </c>
+      <c r="B4">
+        <v>1.84E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0.02</v>
+      </c>
+      <c r="B5">
+        <v>1.8700000000000001E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1.9900000000000001E-2</v>
+      </c>
+      <c r="B6">
+        <v>1.9E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1.9599999999999999E-2</v>
+      </c>
+      <c r="B7">
+        <v>1.95E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1.9800000000000002E-2</v>
+      </c>
+      <c r="B8">
+        <v>1.9599999999999999E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1.9599999999999999E-2</v>
+      </c>
+      <c r="B9">
+        <v>1.95E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>0.02</v>
+      </c>
+      <c r="B10">
+        <v>1.9599999999999999E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>0.02</v>
+      </c>
+      <c r="B11">
+        <v>1.9560000000000001E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f>AVERAGE(A2:A11)</f>
+        <v>1.983E-2</v>
+      </c>
+      <c r="B12">
+        <f>AVERAGE(B2:B11)</f>
+        <v>1.9206000000000001E-2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f>STDEV(A2:A11)</f>
+        <v>1.7669811040931473E-4</v>
+      </c>
+      <c r="B13">
+        <f>STDEV(B2:B11)</f>
+        <v>4.2153687066890516E-4</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f>((A12-(C1))/(C1))*100</f>
+        <v>-0.84702541076232329</v>
+      </c>
+      <c r="B14">
+        <f>(B12-C1)/(C1)*100</f>
+        <v>-3.9671190135704055</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f>A13*100/A12</f>
+        <v>0.89106460115640307</v>
+      </c>
+      <c r="B15">
+        <f>B13*100/B12</f>
+        <v>2.1948186539045356</v>
+      </c>
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1">
+        <f>0.05*0.99997</f>
+        <v>4.9998500000000001E-2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>4.9599999999999998E-2</v>
+      </c>
+      <c r="B2">
+        <v>5.7099999999999998E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>4.9799999999999997E-2</v>
+      </c>
+      <c r="B3">
+        <v>5.4600000000000003E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4.9799999999999997E-2</v>
+      </c>
+      <c r="B4">
+        <v>5.3499999999999999E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0.05</v>
+      </c>
+      <c r="B5">
+        <v>5.3999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5.0099999999999999E-2</v>
+      </c>
+      <c r="B6">
+        <v>5.4699999999999999E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>0.05</v>
+      </c>
+      <c r="B7">
+        <v>5.16E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>4.99E-2</v>
+      </c>
+      <c r="B8">
+        <v>5.1400000000000001E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>4.99E-2</v>
+      </c>
+      <c r="B9">
+        <v>5.1700000000000003E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>4.99E-2</v>
+      </c>
+      <c r="B10">
+        <v>5.16E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>0.05</v>
+      </c>
+      <c r="B11">
+        <v>5.1299999999999998E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f>AVERAGE(A2:A11)</f>
+        <v>4.99E-2</v>
+      </c>
+      <c r="B12">
+        <f>AVERAGE(B2:B11)</f>
+        <v>5.3149999999999996E-2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f>STDEV(A2:A11)</f>
+        <v>1.4142135623731081E-4</v>
+      </c>
+      <c r="B13">
+        <f>STDEV(B2:B11)</f>
+        <v>1.953486910913689E-3</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f>((A12-(C1))/(C1))*100</f>
+        <v>-0.19700591017730806</v>
+      </c>
+      <c r="B14">
+        <f>(B12-C1)/(C1)*100</f>
+        <v>6.3031890956728596</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f>A13*100/A12</f>
+        <v>0.28340953153769699</v>
+      </c>
+      <c r="B15">
+        <f>B13*100/B12</f>
+        <v>3.6754222218507793</v>
+      </c>
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>